<commit_message>
memperbaiki struktur file Unit testing.xlsx
</commit_message>
<xml_diff>
--- a/Unit testing.xlsx
+++ b/Unit testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\RPL-Unit-Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0DA3F6-A222-4805-94B4-F20586FE5AD7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8F7282-B8DC-443A-A324-67912B730BD4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t>Module Name:</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Rajkumar</t>
-  </si>
-  <si>
     <t>STATUS 
 (PASS/FAIL)</t>
   </si>
@@ -80,9 +74,6 @@
   <si>
     <t>EXPECTED 
 RESULT</t>
-  </si>
-  <si>
-    <t>Google Email</t>
   </si>
   <si>
     <t>www.SoftwareTestingMaterial.com</t>
@@ -1283,6 +1274,15 @@
   <si>
     <t>Verifikasi form update</t>
   </si>
+  <si>
+    <t>Ardhy, Digdo, Irvan, Razi</t>
+  </si>
+  <si>
+    <t>Penjualan</t>
+  </si>
+  <si>
+    <t>Warung</t>
+  </si>
 </sst>
 </file>
 
@@ -2035,6 +2035,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2047,6 +2059,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2090,21 +2105,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2543,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K748"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59:H64"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2564,102 +2564,102 @@
   <sheetData>
     <row r="1" spans="2:11" ht="5.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="28"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="36"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="35" t="s">
+      <c r="C4" s="27"/>
+      <c r="D4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="36"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="35" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="30"/>
-      <c r="K5" s="31"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="36"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="35" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="35" t="s">
+      <c r="C7" s="27"/>
+      <c r="D7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="9" spans="2:11" ht="41.4" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2681,1399 +2681,1399 @@
         <v>12</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="J9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="2:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="17"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="21"/>
       <c r="F11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="17" t="s">
+      <c r="G14" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+    </row>
+    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="21"/>
+      <c r="C17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="D17" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="21"/>
+      <c r="F17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+    </row>
+    <row r="18" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-    </row>
-    <row r="13" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="18"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18"/>
-    </row>
-    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-    </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
     </row>
     <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="17"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="21"/>
       <c r="F23" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G23" s="3"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
     </row>
     <row r="24" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
+        <v>42</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
       <c r="F25" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
+        <v>20</v>
+      </c>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
       <c r="F26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+    </row>
+    <row r="27" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="22"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+    </row>
+    <row r="29" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="21"/>
+      <c r="F29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="9"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+    </row>
+    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" s="25"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+    </row>
+    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G31" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" s="25"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+    </row>
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="25"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+    </row>
+    <row r="33" spans="2:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H33" s="25"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="17"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="2:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="26"/>
+      <c r="C35" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" s="26"/>
+      <c r="F35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="26"/>
+    </row>
+    <row r="36" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="26"/>
+    </row>
+    <row r="37" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G37" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="26"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="26"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+    </row>
+    <row r="40" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+    </row>
+    <row r="41" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="21"/>
+      <c r="C41" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="21"/>
+      <c r="F41" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+    </row>
+    <row r="42" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
+      <c r="F42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H42" s="22"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+    </row>
+    <row r="43" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+    </row>
+    <row r="44" spans="2:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
+      <c r="F45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="22"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+    </row>
+    <row r="47" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="22"/>
+      <c r="C47" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-    </row>
-    <row r="27" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="3" t="s">
+      <c r="E47" s="21"/>
+      <c r="F47" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G47" s="9"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+    </row>
+    <row r="48" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="22"/>
+    </row>
+    <row r="49" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G49" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G50" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+    </row>
+    <row r="51" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G51" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G52" s="13"/>
+      <c r="H52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
+      <c r="K52" s="22"/>
+    </row>
+    <row r="53" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="21"/>
+      <c r="C53" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="21"/>
+      <c r="F53" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G53" s="9"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="21"/>
+    </row>
+    <row r="54" spans="2:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G54" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="3" t="s">
+      <c r="H54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
+      <c r="K54" s="22"/>
+    </row>
+    <row r="55" spans="2:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
+      <c r="F55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="22"/>
+    </row>
+    <row r="56" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="H56" s="22"/>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+    </row>
+    <row r="57" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
+      <c r="K57" s="22"/>
+    </row>
+    <row r="58" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+    </row>
+    <row r="59" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B59" s="21"/>
+      <c r="C59" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E59" s="21"/>
+      <c r="F59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="21"/>
+    </row>
+    <row r="60" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-    </row>
-    <row r="29" spans="1:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="17"/>
-      <c r="C29" s="17" t="s">
+      <c r="G60" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
+      <c r="F61" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61" s="22"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+      <c r="K61" s="22"/>
+    </row>
+    <row r="62" spans="2:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
+      <c r="F62" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H62" s="22"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
+      <c r="K62" s="22"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="23"/>
+      <c r="I64" s="23"/>
+      <c r="J64" s="23"/>
+      <c r="K64" s="23"/>
+    </row>
+    <row r="65" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B65" s="21"/>
+      <c r="C65" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E65" s="21"/>
+      <c r="F65" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G65" s="9"/>
+      <c r="H65" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I65" s="21"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="21"/>
+    </row>
+    <row r="66" spans="2:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
+      <c r="F66" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G66" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+    </row>
+    <row r="67" spans="2:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="22"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+      <c r="K67" s="22"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
+      <c r="F68" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H68" s="22"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+      <c r="K68" s="22"/>
+    </row>
+    <row r="69" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G69" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="6" t="s">
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+      <c r="K69" s="22"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B70" s="23"/>
+      <c r="C70" s="23"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70" s="16"/>
+      <c r="H70" s="23"/>
+      <c r="I70" s="23"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="23"/>
+    </row>
+    <row r="71" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B71" s="21"/>
+      <c r="C71" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E71" s="21"/>
+      <c r="F71" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G71" s="9"/>
+      <c r="H71" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I71" s="21"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="21"/>
+    </row>
+    <row r="72" spans="2:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
+      <c r="F72" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
+      <c r="K72" s="22"/>
+    </row>
+    <row r="73" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
+      <c r="F73" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
+      <c r="K73" s="22"/>
+    </row>
+    <row r="74" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="9"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
-    </row>
-    <row r="30" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="7" t="s">
+      <c r="G74" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
+      <c r="K74" s="22"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
+      <c r="F75" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G75" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-    </row>
-    <row r="31" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="14" t="s">
+      <c r="H75" s="22"/>
+      <c r="I75" s="22"/>
+      <c r="J75" s="22"/>
+      <c r="K75" s="22"/>
+    </row>
+    <row r="76" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="22"/>
+      <c r="C76" s="23"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
+      <c r="F76" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G76" s="18"/>
+      <c r="H76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="22"/>
+    </row>
+    <row r="77" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="21"/>
+      <c r="C77" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="21"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-    </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H32" s="21"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-    </row>
-    <row r="33" spans="2:11" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="5" t="s">
+      <c r="D77" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E77" s="21"/>
+      <c r="F77" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="G77" s="3"/>
+      <c r="H77" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="21"/>
+    </row>
+    <row r="78" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" s="22"/>
+      <c r="I78" s="22"/>
+      <c r="J78" s="22"/>
+      <c r="K78" s="22"/>
+    </row>
+    <row r="79" spans="2:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
+      <c r="F79" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-    </row>
-    <row r="34" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="5" t="s">
+      <c r="G79" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H79" s="22"/>
+      <c r="I79" s="22"/>
+      <c r="J79" s="22"/>
+      <c r="K79" s="22"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G80" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="22"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G81" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H81" s="22"/>
+      <c r="I81" s="22"/>
+      <c r="J81" s="22"/>
+      <c r="K81" s="22"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G82" s="7"/>
+      <c r="H82" s="23"/>
+      <c r="I82" s="23"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="23"/>
+    </row>
+    <row r="83" spans="2:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B83" s="26"/>
+      <c r="C83" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D83" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E83" s="26"/>
+      <c r="F83" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G83" s="3"/>
+      <c r="H83" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="I83" s="26"/>
+      <c r="J83" s="26"/>
+      <c r="K83" s="26"/>
+    </row>
+    <row r="84" spans="2:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="26"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="26"/>
+      <c r="E84" s="26"/>
+      <c r="F84" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G34" s="36"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="18"/>
-    </row>
-    <row r="35" spans="2:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="37"/>
-      <c r="C35" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D35" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="3" t="s">
+      <c r="G84" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H84" s="26"/>
+      <c r="I84" s="26"/>
+      <c r="J84" s="26"/>
+      <c r="K84" s="26"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B85" s="26"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="26"/>
+      <c r="E85" s="26"/>
+      <c r="F85" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H85" s="26"/>
+      <c r="I85" s="26"/>
+      <c r="J85" s="26"/>
+      <c r="K85" s="26"/>
+    </row>
+    <row r="86" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="26"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="26"/>
+      <c r="E86" s="26"/>
+      <c r="F86" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="37"/>
-      <c r="I35" s="37"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="37"/>
-    </row>
-    <row r="36" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="37"/>
-      <c r="E36" s="37"/>
-      <c r="F36" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="37"/>
-      <c r="I36" s="37"/>
-      <c r="J36" s="37"/>
-      <c r="K36" s="37"/>
-    </row>
-    <row r="37" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="37"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G37" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="37"/>
-      <c r="K37" s="37"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
-      <c r="J38" s="37"/>
-      <c r="K38" s="37"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="3" t="s">
+      <c r="G86" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H86" s="26"/>
+      <c r="I86" s="26"/>
+      <c r="J86" s="26"/>
+      <c r="K86" s="26"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B87" s="26"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="26"/>
+      <c r="E87" s="26"/>
+      <c r="F87" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H87" s="26"/>
+      <c r="I87" s="26"/>
+      <c r="J87" s="26"/>
+      <c r="K87" s="26"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B88" s="26"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="26"/>
+      <c r="E88" s="26"/>
+      <c r="F88" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G88" s="7"/>
+      <c r="H88" s="26"/>
+      <c r="I88" s="26"/>
+      <c r="J88" s="26"/>
+      <c r="K88" s="26"/>
+    </row>
+    <row r="89" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B89" s="21"/>
+      <c r="C89" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D89" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="E89" s="21"/>
+      <c r="F89" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G89" s="9"/>
+      <c r="H89" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="I89" s="21"/>
+      <c r="J89" s="21"/>
+      <c r="K89" s="21"/>
+    </row>
+    <row r="90" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H90" s="22"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="22"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-    </row>
-    <row r="40" spans="2:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G40" s="7"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-    </row>
-    <row r="41" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="17"/>
-      <c r="C41" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="3" t="s">
+      <c r="G91" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="22"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17"/>
-      <c r="K41" s="17"/>
-    </row>
-    <row r="42" spans="2:11" ht="12" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-    </row>
-    <row r="43" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-    </row>
-    <row r="44" spans="2:11" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44" s="18"/>
-      <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H45" s="18"/>
-      <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="18"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B46" s="19"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="19"/>
-      <c r="I46" s="19"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
-    </row>
-    <row r="47" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="18"/>
-      <c r="C47" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D47" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="G47" s="9"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-    </row>
-    <row r="48" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-    </row>
-    <row r="49" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B50" s="18"/>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-      <c r="F50" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H50" s="18"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-    </row>
-    <row r="51" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="18"/>
-      <c r="C51" s="18"/>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-      <c r="F52" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G52" s="13"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="18"/>
-    </row>
-    <row r="53" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B53" s="17"/>
-      <c r="C53" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G53" s="9"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="17"/>
-    </row>
-    <row r="54" spans="2:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="18"/>
-      <c r="C54" s="18"/>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-    </row>
-    <row r="55" spans="2:11" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-      <c r="F55" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H55" s="18"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="18"/>
-    </row>
-    <row r="56" spans="2:11" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="18"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="18"/>
-      <c r="E56" s="18"/>
-      <c r="F56" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H56" s="18"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-    </row>
-    <row r="57" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H57" s="18"/>
-      <c r="I57" s="18"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-    </row>
-    <row r="58" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G58" s="7"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-    </row>
-    <row r="59" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B59" s="17"/>
-      <c r="C59" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G59" s="3"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
-      <c r="J59" s="17"/>
-      <c r="K59" s="17"/>
-    </row>
-    <row r="60" spans="2:11" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B61" s="18"/>
-      <c r="C61" s="18"/>
-      <c r="D61" s="18"/>
-      <c r="E61" s="18"/>
-      <c r="F61" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H61" s="18"/>
-      <c r="I61" s="18"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="18"/>
-    </row>
-    <row r="62" spans="2:11" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H62" s="18"/>
-      <c r="I62" s="18"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
-      <c r="F63" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H63" s="18"/>
-      <c r="I63" s="18"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="18"/>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B64" s="19"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G64" s="7"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-    </row>
-    <row r="65" spans="2:11" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="17"/>
-      <c r="C65" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="E65" s="17"/>
-      <c r="F65" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G65" s="9"/>
-      <c r="H65" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-    </row>
-    <row r="66" spans="2:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="18"/>
-      <c r="C66" s="18"/>
-      <c r="D66" s="18"/>
-      <c r="E66" s="18"/>
-      <c r="F66" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H66" s="18"/>
-      <c r="I66" s="18"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="18"/>
-    </row>
-    <row r="67" spans="2:11" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="18"/>
-      <c r="E67" s="18"/>
-      <c r="F67" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H67" s="18"/>
-      <c r="I67" s="18"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-    </row>
-    <row r="69" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
-      <c r="F69" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G69" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="19"/>
-      <c r="E70" s="19"/>
-      <c r="F70" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G70" s="16"/>
-      <c r="H70" s="19"/>
-      <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
-      <c r="K70" s="19"/>
-    </row>
-    <row r="71" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B71" s="17"/>
-      <c r="C71" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E71" s="17"/>
-      <c r="F71" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G71" s="9"/>
-      <c r="H71" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I71" s="17"/>
-      <c r="J71" s="17"/>
-      <c r="K71" s="17"/>
-    </row>
-    <row r="72" spans="2:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G72" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="H72" s="18"/>
-      <c r="I72" s="18"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="18"/>
-    </row>
-    <row r="73" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
-      <c r="D73" s="18"/>
-      <c r="E73" s="18"/>
-      <c r="F73" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H73" s="18"/>
-      <c r="I73" s="18"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="18"/>
-    </row>
-    <row r="74" spans="2:11" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G74" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="18"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H75" s="18"/>
-      <c r="I75" s="18"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="18"/>
-    </row>
-    <row r="76" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="18"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="18"/>
-      <c r="E76" s="18"/>
-      <c r="F76" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G76" s="38"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-    </row>
-    <row r="77" spans="2:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="17"/>
-      <c r="C77" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D77" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E77" s="17"/>
-      <c r="F77" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G77" s="3"/>
-      <c r="H77" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I77" s="17"/>
-      <c r="J77" s="17"/>
-      <c r="K77" s="17"/>
-    </row>
-    <row r="78" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B78" s="18"/>
-      <c r="C78" s="18"/>
-      <c r="D78" s="18"/>
-      <c r="E78" s="18"/>
-      <c r="F78" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H78" s="18"/>
-      <c r="I78" s="18"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="18"/>
-    </row>
-    <row r="79" spans="2:11" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18"/>
-      <c r="E79" s="18"/>
-      <c r="F79" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H79" s="18"/>
-      <c r="I79" s="18"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="18"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B80" s="18"/>
-      <c r="C80" s="18"/>
-      <c r="D80" s="18"/>
-      <c r="E80" s="18"/>
-      <c r="F80" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H80" s="18"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="18"/>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B81" s="18"/>
-      <c r="C81" s="18"/>
-      <c r="D81" s="18"/>
-      <c r="E81" s="18"/>
-      <c r="F81" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G81" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H81" s="18"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="18"/>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G82" s="7"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-      <c r="J82" s="19"/>
-      <c r="K82" s="19"/>
-    </row>
-    <row r="83" spans="2:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B83" s="37"/>
-      <c r="C83" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D83" s="37" t="s">
+      <c r="G92" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+    </row>
+    <row r="93" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G93" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E83" s="37"/>
-      <c r="F83" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G83" s="3"/>
-      <c r="H83" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="I83" s="37"/>
-      <c r="J83" s="37"/>
-      <c r="K83" s="37"/>
-    </row>
-    <row r="84" spans="2:11" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="37"/>
-      <c r="C84" s="18"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H84" s="37"/>
-      <c r="I84" s="37"/>
-      <c r="J84" s="37"/>
-      <c r="K84" s="37"/>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B85" s="37"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H85" s="37"/>
-      <c r="I85" s="37"/>
-      <c r="J85" s="37"/>
-      <c r="K85" s="37"/>
-    </row>
-    <row r="86" spans="2:11" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="37"/>
-      <c r="C86" s="18"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H86" s="37"/>
-      <c r="I86" s="37"/>
-      <c r="J86" s="37"/>
-      <c r="K86" s="37"/>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B87" s="37"/>
-      <c r="C87" s="18"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H87" s="37"/>
-      <c r="I87" s="37"/>
-      <c r="J87" s="37"/>
-      <c r="K87" s="37"/>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B88" s="37"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G88" s="7"/>
-      <c r="H88" s="37"/>
-      <c r="I88" s="37"/>
-      <c r="J88" s="37"/>
-      <c r="K88" s="37"/>
-    </row>
-    <row r="89" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B89" s="17"/>
-      <c r="C89" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D89" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E89" s="17"/>
-      <c r="F89" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G89" s="9"/>
-      <c r="H89" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I89" s="17"/>
-      <c r="J89" s="17"/>
-      <c r="K89" s="17"/>
-    </row>
-    <row r="90" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H90" s="18"/>
-      <c r="I90" s="18"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="18"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B91" s="18"/>
-      <c r="C91" s="18"/>
-      <c r="D91" s="18"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G91" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="18"/>
-      <c r="K91" s="18"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B92" s="18"/>
-      <c r="C92" s="18"/>
-      <c r="D92" s="18"/>
-      <c r="E92" s="18"/>
-      <c r="F92" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G92" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="H92" s="18"/>
-      <c r="I92" s="18"/>
-      <c r="J92" s="18"/>
-      <c r="K92" s="18"/>
-    </row>
-    <row r="93" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B93" s="18"/>
-      <c r="C93" s="18"/>
-      <c r="D93" s="18"/>
-      <c r="E93" s="18"/>
-      <c r="F93" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="G93" s="39" t="s">
-        <v>41</v>
-      </c>
-      <c r="H93" s="18"/>
-      <c r="I93" s="18"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="18"/>
+      <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B94" s="18"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="18"/>
-      <c r="E94" s="18"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
       <c r="F94" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G94" s="40"/>
-      <c r="H94" s="18"/>
-      <c r="I94" s="18"/>
-      <c r="J94" s="18"/>
-      <c r="K94" s="18"/>
+        <v>56</v>
+      </c>
+      <c r="G94" s="20"/>
+      <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="22"/>
+      <c r="K94" s="22"/>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B95" s="2"/>
@@ -4135,7 +4135,7 @@
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
     </row>
-    <row r="100" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -11925,111 +11925,6 @@
     </row>
   </sheetData>
   <mergeCells count="125">
-    <mergeCell ref="B65:B70"/>
-    <mergeCell ref="C65:C70"/>
-    <mergeCell ref="D65:D70"/>
-    <mergeCell ref="E65:E70"/>
-    <mergeCell ref="H65:H70"/>
-    <mergeCell ref="I65:I70"/>
-    <mergeCell ref="J65:J70"/>
-    <mergeCell ref="K65:K70"/>
-    <mergeCell ref="B71:B76"/>
-    <mergeCell ref="C71:C76"/>
-    <mergeCell ref="D71:D76"/>
-    <mergeCell ref="E71:E76"/>
-    <mergeCell ref="H71:H76"/>
-    <mergeCell ref="I71:I76"/>
-    <mergeCell ref="J71:J76"/>
-    <mergeCell ref="K71:K76"/>
-    <mergeCell ref="B77:B82"/>
-    <mergeCell ref="C77:C82"/>
-    <mergeCell ref="D77:D82"/>
-    <mergeCell ref="E77:E82"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="D41:D46"/>
-    <mergeCell ref="E41:E46"/>
-    <mergeCell ref="H41:H46"/>
-    <mergeCell ref="I41:I46"/>
-    <mergeCell ref="J41:J46"/>
-    <mergeCell ref="K41:K46"/>
-    <mergeCell ref="B47:B52"/>
-    <mergeCell ref="C47:C52"/>
-    <mergeCell ref="D47:D52"/>
-    <mergeCell ref="E47:E52"/>
-    <mergeCell ref="H47:H52"/>
-    <mergeCell ref="I47:I52"/>
-    <mergeCell ref="J47:J52"/>
-    <mergeCell ref="K47:K52"/>
-    <mergeCell ref="H29:H34"/>
-    <mergeCell ref="I29:I34"/>
-    <mergeCell ref="J29:J34"/>
-    <mergeCell ref="K29:K34"/>
-    <mergeCell ref="B35:B40"/>
-    <mergeCell ref="C35:C40"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="E35:E40"/>
-    <mergeCell ref="H35:H40"/>
-    <mergeCell ref="I35:I40"/>
-    <mergeCell ref="J35:J40"/>
-    <mergeCell ref="K35:K40"/>
-    <mergeCell ref="B23:B28"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="D23:D28"/>
-    <mergeCell ref="E23:E28"/>
-    <mergeCell ref="H23:H28"/>
-    <mergeCell ref="I23:I28"/>
-    <mergeCell ref="J23:J28"/>
-    <mergeCell ref="K23:K28"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="D29:D34"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="H17:H22"/>
-    <mergeCell ref="I17:I22"/>
-    <mergeCell ref="J17:J22"/>
-    <mergeCell ref="K17:K22"/>
-    <mergeCell ref="B11:B16"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="D11:D16"/>
-    <mergeCell ref="E11:E16"/>
-    <mergeCell ref="H11:H16"/>
-    <mergeCell ref="I11:I16"/>
-    <mergeCell ref="J11:J16"/>
-    <mergeCell ref="K11:K16"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:K7"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="E29:E34"/>
-    <mergeCell ref="B59:B64"/>
-    <mergeCell ref="C59:C64"/>
-    <mergeCell ref="D59:D64"/>
-    <mergeCell ref="E59:E64"/>
-    <mergeCell ref="H59:H64"/>
-    <mergeCell ref="I59:I64"/>
-    <mergeCell ref="J59:J64"/>
-    <mergeCell ref="K59:K64"/>
-    <mergeCell ref="B83:B88"/>
-    <mergeCell ref="C83:C88"/>
-    <mergeCell ref="D83:D88"/>
-    <mergeCell ref="E83:E88"/>
-    <mergeCell ref="H83:H88"/>
-    <mergeCell ref="I83:I88"/>
-    <mergeCell ref="J83:J88"/>
-    <mergeCell ref="K83:K88"/>
     <mergeCell ref="E89:E94"/>
     <mergeCell ref="D89:D94"/>
     <mergeCell ref="C89:C94"/>
@@ -12050,6 +11945,111 @@
     <mergeCell ref="I77:I82"/>
     <mergeCell ref="J77:J82"/>
     <mergeCell ref="K77:K82"/>
+    <mergeCell ref="I59:I64"/>
+    <mergeCell ref="J59:J64"/>
+    <mergeCell ref="K59:K64"/>
+    <mergeCell ref="B83:B88"/>
+    <mergeCell ref="C83:C88"/>
+    <mergeCell ref="D83:D88"/>
+    <mergeCell ref="E83:E88"/>
+    <mergeCell ref="H83:H88"/>
+    <mergeCell ref="I83:I88"/>
+    <mergeCell ref="J83:J88"/>
+    <mergeCell ref="K83:K88"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:K7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="H17:H22"/>
+    <mergeCell ref="I17:I22"/>
+    <mergeCell ref="J17:J22"/>
+    <mergeCell ref="K17:K22"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="I11:I16"/>
+    <mergeCell ref="J11:J16"/>
+    <mergeCell ref="K11:K16"/>
+    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="D23:D28"/>
+    <mergeCell ref="E23:E28"/>
+    <mergeCell ref="H23:H28"/>
+    <mergeCell ref="I23:I28"/>
+    <mergeCell ref="J23:J28"/>
+    <mergeCell ref="K23:K28"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="D29:D34"/>
+    <mergeCell ref="E29:E34"/>
+    <mergeCell ref="H29:H34"/>
+    <mergeCell ref="I29:I34"/>
+    <mergeCell ref="J29:J34"/>
+    <mergeCell ref="K29:K34"/>
+    <mergeCell ref="B35:B40"/>
+    <mergeCell ref="C35:C40"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="E35:E40"/>
+    <mergeCell ref="H35:H40"/>
+    <mergeCell ref="I35:I40"/>
+    <mergeCell ref="J35:J40"/>
+    <mergeCell ref="K35:K40"/>
+    <mergeCell ref="I41:I46"/>
+    <mergeCell ref="J41:J46"/>
+    <mergeCell ref="K41:K46"/>
+    <mergeCell ref="B47:B52"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="D47:D52"/>
+    <mergeCell ref="E47:E52"/>
+    <mergeCell ref="H47:H52"/>
+    <mergeCell ref="I47:I52"/>
+    <mergeCell ref="J47:J52"/>
+    <mergeCell ref="K47:K52"/>
+    <mergeCell ref="B77:B82"/>
+    <mergeCell ref="C77:C82"/>
+    <mergeCell ref="D77:D82"/>
+    <mergeCell ref="E77:E82"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="D41:D46"/>
+    <mergeCell ref="E41:E46"/>
+    <mergeCell ref="H41:H46"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="C59:C64"/>
+    <mergeCell ref="D59:D64"/>
+    <mergeCell ref="E59:E64"/>
+    <mergeCell ref="H59:H64"/>
+    <mergeCell ref="B65:B70"/>
+    <mergeCell ref="C65:C70"/>
+    <mergeCell ref="D65:D70"/>
+    <mergeCell ref="E65:E70"/>
+    <mergeCell ref="H65:H70"/>
+    <mergeCell ref="I65:I70"/>
+    <mergeCell ref="J65:J70"/>
+    <mergeCell ref="K65:K70"/>
+    <mergeCell ref="B71:B76"/>
+    <mergeCell ref="C71:C76"/>
+    <mergeCell ref="D71:D76"/>
+    <mergeCell ref="E71:E76"/>
+    <mergeCell ref="H71:H76"/>
+    <mergeCell ref="I71:I76"/>
+    <mergeCell ref="J71:J76"/>
+    <mergeCell ref="K71:K76"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>